<commit_message>
Atualizacao documentacao de gerencia de projeto
</commit_message>
<xml_diff>
--- a/academicci_documentacao/gerencia_projeto/Academicci_LR_Riscos.xlsx
+++ b/academicci_documentacao/gerencia_projeto/Academicci_LR_Riscos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Google Drive\University - Atividades e Trabalhos\PFS_II\repositorio\documentacao\gerencia_projeto\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Raphael\Google Drive\University - Atividades e Trabalhos\PFS_II\Academicci_II\academicci_documentacao\gerencia_projeto\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -168,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="48">
   <si>
     <t>ID Risco</t>
   </si>
@@ -196,9 +196,6 @@
   <si>
     <t>Data 
 Identificação</t>
-  </si>
-  <si>
-    <t>&lt;projeto&gt; Lista de Riscos</t>
   </si>
   <si>
     <t>Categoria</t>
@@ -251,6 +248,77 @@
   </si>
   <si>
     <t>Buscar formas da equipe aprender progamação</t>
+  </si>
+  <si>
+    <t>Academicci - Lista de Riscos</t>
+  </si>
+  <si>
+    <t>Alteração nos Requisitos</t>
+  </si>
+  <si>
+    <t>Dependência do usuário professor</t>
+  </si>
+  <si>
+    <t>Conhecimento técnico do time de desenvolvimento</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Defeitos no software não encontrados antes da implantação </t>
+  </si>
+  <si>
+    <t>Devido aos requisitos já implementados há uma dificuldade na implementação e adapatação de novos requisitos</t>
+  </si>
+  <si>
+    <t>Devido à grande responsabilidade de execução de tarefas no sistema pelo usuário, podem gerar travamentos de atividades aos alunos-monitores.</t>
+  </si>
+  <si>
+    <t>Devido ao fato que nem todos os integrantes do time de desenvolvimento possuem habilidade técnica de programação e desenvolvimento, isso pode acarretar em sobrecarga a membros e/ou atraso na entrega</t>
+  </si>
+  <si>
+    <t>Devido a ausência ou aplicação falha de testes durante a implementação do sistema, podem vir a ocorrer defeitos após a entrega das releases</t>
+  </si>
+  <si>
+    <t>Externa</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Time de Desenvolvimento</t>
+  </si>
+  <si>
+    <t>Fuga</t>
+  </si>
+  <si>
+    <t>Realizar planenejamento detalhado para preparar o projeto às possíveis mudanças de requisitos.</t>
+  </si>
+  <si>
+    <t>Elaborar treinamento aos docentes e implementar processo de notificações para que o docente seja lembrando de executar as ações.</t>
+  </si>
+  <si>
+    <t>* Promover capacitação técnica à equipe 
+* Fornecer Plano de Aprendizado à equipe</t>
+  </si>
+  <si>
+    <t>Falta de Organização na Equipe</t>
+  </si>
+  <si>
+    <t>Devido a falta de uma estrutura sólida da equipe pode haver falta de organização na equipe</t>
+  </si>
+  <si>
+    <t>Gestão de Projeto</t>
+  </si>
+  <si>
+    <t>Scrum Master</t>
+  </si>
+  <si>
+    <t>Product Owner</t>
+  </si>
+  <si>
+    <t>* Melhorar a comunicação da Equipe
+* Promover mudança de cultura na organização da equipe</t>
+  </si>
+  <si>
+    <t>Elaborar um plano de testes, e exectar todos os testes necessários antes de disponibilizar o sistema ao usuário.</t>
   </si>
 </sst>
 </file>
@@ -260,7 +328,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -299,6 +367,11 @@
       <sz val="9"/>
       <color indexed="81"/>
       <name val="Segoe UI"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -346,7 +419,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -360,9 +433,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -383,6 +453,18 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -701,42 +783,42 @@
   <dimension ref="A1:AC113"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="94" zoomScaleNormal="94" workbookViewId="0">
-      <selection activeCell="M5" sqref="M5"/>
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="3.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="61" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="7" max="9" width="3.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="5.42578125" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="4.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="23.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="12.7109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="36.140625" style="1" customWidth="1"/>
+    <col min="13" max="13" width="53.5703125" style="1" customWidth="1"/>
     <col min="14" max="29" width="9.140625" style="1"/>
     <col min="30" max="16384" width="9.140625" style="2"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" ht="23.25" x14ac:dyDescent="0.35">
-      <c r="A1" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
-      <c r="E1" s="9"/>
-      <c r="F1" s="9"/>
-      <c r="G1" s="9"/>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
-      <c r="J1" s="9"/>
-      <c r="K1" s="9"/>
-      <c r="L1" s="9"/>
-      <c r="M1" s="9"/>
+      <c r="A1" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="16"/>
+      <c r="E1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
+      <c r="L1" s="16"/>
+      <c r="M1" s="16"/>
     </row>
     <row r="2" spans="1:13" ht="72.75" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
@@ -749,13 +831,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G2" s="3" t="s">
         <v>3</v>
@@ -769,75 +851,75 @@
       <c r="J2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="16" t="s">
+      <c r="K2" s="15" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="M2" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="38.25" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
+        <v>1</v>
+      </c>
+      <c r="B3" s="13">
+        <v>43136</v>
+      </c>
+      <c r="C3" s="9" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="3" spans="1:13" ht="51" x14ac:dyDescent="0.2">
-      <c r="A3" s="10">
-        <v>1</v>
-      </c>
-      <c r="B3" s="14">
-        <v>43136</v>
-      </c>
-      <c r="C3" s="10" t="s">
+      <c r="D3" s="9"/>
+      <c r="E3" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D3" s="10"/>
-      <c r="E3" s="15" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="10" t="s">
+      <c r="G3" s="10" t="s">
         <v>15</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H3" s="10">
+      <c r="H3" s="9">
         <v>5</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="9">
         <v>4</v>
       </c>
-      <c r="J3" s="13">
+      <c r="J3" s="12">
         <f>+H3*I3</f>
         <v>20</v>
       </c>
-      <c r="K3" s="10" t="s">
+      <c r="K3" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="L3" s="19" t="s">
         <v>17</v>
       </c>
-      <c r="L3" s="10" t="s">
+      <c r="M3" s="11" t="s">
         <v>18</v>
-      </c>
-      <c r="M3" s="12" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="6">
         <v>2</v>
       </c>
-      <c r="B4" s="14">
+      <c r="B4" s="13">
         <v>43136</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>21</v>
+      <c r="C4" s="9" t="s">
+        <v>20</v>
       </c>
       <c r="D4" s="6"/>
       <c r="E4" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H4" s="6">
         <v>5</v>
@@ -850,120 +932,220 @@
         <v>25</v>
       </c>
       <c r="K4" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="L4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="L4" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M4" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="M4" s="6" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:13" ht="30" x14ac:dyDescent="0.2">
       <c r="A5" s="6">
         <v>3</v>
       </c>
-      <c r="B5" s="14"/>
-      <c r="C5" s="6"/>
+      <c r="B5" s="13">
+        <v>42999</v>
+      </c>
+      <c r="C5" s="17" t="s">
+        <v>26</v>
+      </c>
       <c r="D5" s="6"/>
-      <c r="E5" s="6"/>
-      <c r="F5" s="6"/>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6"/>
+      <c r="E5" s="18" t="s">
+        <v>30</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H5" s="6">
+        <v>3</v>
+      </c>
+      <c r="I5" s="6">
+        <v>6</v>
+      </c>
       <c r="J5" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K5" s="6"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="6"/>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+        <v>18</v>
+      </c>
+      <c r="K5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A6" s="6">
         <v>4</v>
       </c>
-      <c r="B6" s="14"/>
-      <c r="C6" s="6"/>
+      <c r="B6" s="13">
+        <v>42999</v>
+      </c>
+      <c r="C6" s="17" t="s">
+        <v>27</v>
+      </c>
       <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
+      <c r="E6" s="18" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="6">
+        <v>6</v>
+      </c>
       <c r="J6" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="6"/>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="K6" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="L6" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="60" x14ac:dyDescent="0.2">
       <c r="A7" s="6">
         <v>5</v>
       </c>
-      <c r="B7" s="14"/>
-      <c r="C7" s="6"/>
+      <c r="B7" s="13">
+        <v>42999</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>28</v>
+      </c>
       <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
-      <c r="F7" s="6"/>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
+      <c r="E7" s="18" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H7" s="6">
+        <v>5</v>
+      </c>
+      <c r="I7" s="6">
+        <v>7</v>
+      </c>
       <c r="J7" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K7" s="6"/>
-      <c r="L7" s="6"/>
-      <c r="M7" s="6"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+        <v>35</v>
+      </c>
+      <c r="K7" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L7" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="M7" s="18" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="45" x14ac:dyDescent="0.2">
       <c r="A8" s="6">
         <v>6</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="6"/>
+      <c r="B8" s="13">
+        <v>42999</v>
+      </c>
+      <c r="C8" s="18" t="s">
+        <v>29</v>
+      </c>
       <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
+      <c r="E8" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="6">
+        <v>2</v>
+      </c>
+      <c r="I8" s="6">
+        <v>3</v>
+      </c>
       <c r="J8" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K8" s="6"/>
-      <c r="L8" s="6"/>
-      <c r="M8" s="6"/>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+        <v>6</v>
+      </c>
+      <c r="K8" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="L8" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A9" s="6">
         <v>7</v>
       </c>
-      <c r="B9" s="14"/>
-      <c r="C9" s="6"/>
+      <c r="B9" s="13">
+        <v>43161</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>41</v>
+      </c>
       <c r="D9" s="6"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
+      <c r="E9" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="H9" s="6">
+        <v>5</v>
+      </c>
+      <c r="I9" s="6">
+        <v>7</v>
+      </c>
       <c r="J9" s="7">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="K9" s="6"/>
-      <c r="L9" s="6"/>
-      <c r="M9" s="6"/>
+        <v>35</v>
+      </c>
+      <c r="K9" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="L9" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="M9" s="11" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="6">
         <v>8</v>
       </c>
-      <c r="B10" s="14"/>
+      <c r="B10" s="13"/>
       <c r="C10" s="6"/>
       <c r="D10" s="6"/>
       <c r="E10" s="6"/>
@@ -983,7 +1165,7 @@
       <c r="A11" s="6">
         <v>9</v>
       </c>
-      <c r="B11" s="14"/>
+      <c r="B11" s="13"/>
       <c r="C11" s="6"/>
       <c r="D11" s="6"/>
       <c r="E11" s="6"/>
@@ -1003,7 +1185,7 @@
       <c r="A12" s="6">
         <v>10</v>
       </c>
-      <c r="B12" s="14"/>
+      <c r="B12" s="13"/>
       <c r="C12" s="6"/>
       <c r="D12" s="6"/>
       <c r="E12" s="6"/>
@@ -1023,7 +1205,7 @@
       <c r="A13" s="6">
         <v>11</v>
       </c>
-      <c r="B13" s="14"/>
+      <c r="B13" s="13"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
       <c r="E13" s="6"/>
@@ -1043,7 +1225,7 @@
       <c r="A14" s="6">
         <v>12</v>
       </c>
-      <c r="B14" s="14"/>
+      <c r="B14" s="13"/>
       <c r="C14" s="6"/>
       <c r="D14" s="6"/>
       <c r="E14" s="6"/>
@@ -1063,7 +1245,7 @@
       <c r="A15" s="6">
         <v>13</v>
       </c>
-      <c r="B15" s="14"/>
+      <c r="B15" s="13"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
       <c r="E15" s="6"/>
@@ -1083,7 +1265,7 @@
       <c r="A16" s="6">
         <v>14</v>
       </c>
-      <c r="B16" s="14"/>
+      <c r="B16" s="13"/>
       <c r="C16" s="6"/>
       <c r="D16" s="6"/>
       <c r="E16" s="6"/>
@@ -1103,7 +1285,7 @@
       <c r="A17" s="6">
         <v>15</v>
       </c>
-      <c r="B17" s="14"/>
+      <c r="B17" s="13"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
       <c r="E17" s="6"/>
@@ -1123,7 +1305,7 @@
       <c r="A18" s="6">
         <v>16</v>
       </c>
-      <c r="B18" s="14"/>
+      <c r="B18" s="13"/>
       <c r="C18" s="6"/>
       <c r="D18" s="6"/>
       <c r="E18" s="6"/>
@@ -1143,7 +1325,7 @@
       <c r="A19" s="6">
         <v>17</v>
       </c>
-      <c r="B19" s="14"/>
+      <c r="B19" s="13"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
       <c r="E19" s="6"/>
@@ -1163,7 +1345,7 @@
       <c r="A20" s="6">
         <v>18</v>
       </c>
-      <c r="B20" s="14"/>
+      <c r="B20" s="13"/>
       <c r="C20" s="6"/>
       <c r="D20" s="6"/>
       <c r="E20" s="6"/>
@@ -1183,7 +1365,7 @@
       <c r="A21" s="6">
         <v>19</v>
       </c>
-      <c r="B21" s="14"/>
+      <c r="B21" s="13"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -1314,6 +1496,18 @@
   <mergeCells count="1">
     <mergeCell ref="A1:M1"/>
   </mergeCells>
+  <conditionalFormatting sqref="J3:J22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <dataValidations count="2">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G3:G22">
       <formula1>"D,I"</formula1>

</xml_diff>